<commit_message>
Prove the effectiveness of dire-refined word vectors on word level
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,66 +20,222 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
+  <si>
+    <t>sentiment-PCA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.519572063604288 0.5047601413582851</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.0289928313540157 0.028771276958986746</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.12541278905267025 0.11852712367137125</t>
+  </si>
+  <si>
+    <t>0.13602237609896586 0.13659216228024537</t>
+  </si>
+  <si>
+    <t>SSWE_h(50)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SSWE_r(50)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SSWE_u(50)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>simlex-999(pearsonr, spearmanr)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.542532298026846 0.5296450386863069</t>
+  </si>
   <si>
     <t>fastText-crawl-300d-2M.vec</t>
-  </si>
-  <si>
-    <t>[0.28633193 0.11676843 0.09353362 0.07186453 0.06552153 0.05351857</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.0471763  0.04025202 0.03875825 0.03124195]</t>
-  </si>
-  <si>
-    <t>sentiment-PCA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wordsim-999(pearsonr, spearmanr)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.519572063604288 0.5047601413582851</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.0289928313540157 0.028771276958986746</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[0.68817972 0.09736926 0.04696623 0.02594634 0.02426833 0.02200869</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.01670254 0.01552719 0.01180113 0.01062583]</t>
-  </si>
-  <si>
-    <t>[0.63171184 0.11711445 0.06208693 0.03295661 0.02583572 0.02417193</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.01876501 0.01722527 0.01438883 0.01111564]</t>
-  </si>
-  <si>
-    <t>0.12541278905267025 0.11852712367137125</t>
-  </si>
-  <si>
-    <t>0.13602237609896586 0.13659216228024537</t>
-  </si>
-  <si>
-    <t>[0.8134059  0.05878878 0.03315523 0.02614427 0.01813707 0.00998843</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.00779787 0.00627137 0.00506332 0.00470372]</t>
-  </si>
-  <si>
-    <t>SSWE_h(50)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SSWE_r(50)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SSWE_u(50)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>refined(fastText-crawl-300d-2M.vec)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.7329544531192245 0.7780425795462853</t>
+  </si>
+  <si>
+    <t>capital-common-countries.txt:</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 83.20% (421/506)</t>
+  </si>
+  <si>
+    <t>capital-world.txt:</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 72.66% (2105/2897)</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 72.59% (2103/2897)</t>
+  </si>
+  <si>
+    <t>currency.txt:</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 38.70% (291/752)</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 38.16% (287/752)</t>
+  </si>
+  <si>
+    <t>city-in-state.txt:</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 77.10% (1448/1878)</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 77.16% (1449/1878)</t>
+  </si>
+  <si>
+    <t>family.txt:</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 100.00% (342/342)</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 99.71% (341/342)</t>
+  </si>
+  <si>
+    <t>gram1-adjective-to-adverb.txt:</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 38.61% (383/992)</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 36.59% (363/992)</t>
+  </si>
+  <si>
+    <t>gram2-opposite.txt:</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 60.22% (489/812)</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 61.08% (496/812)</t>
+  </si>
+  <si>
+    <t>gram3-comparative.txt:</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 88.97% (242/272)</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 88.60% (241/272)</t>
+  </si>
+  <si>
+    <t>gram4-superlative.txt:</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 100.00% (56/56)</t>
+  </si>
+  <si>
+    <t>gram5-present-participle.txt:</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 93.00% (558/600)</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 92.33% (554/600)</t>
+  </si>
+  <si>
+    <t>gram6-nationality-adjective.txt:</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 81.04% (1111/1371)</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 81.25% (1114/1371)</t>
+  </si>
+  <si>
+    <t>gram7-past-tense.txt:</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 81.37% (249/306)</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 82.68% (253/306)</t>
+  </si>
+  <si>
+    <t>gram8-plural.txt:</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 86.67% (26/30)</t>
+  </si>
+  <si>
+    <t>gram9-plural-verbs.txt:</t>
+  </si>
+  <si>
+    <t>ACCURACY TOP1: 83.33% (5/6)</t>
+  </si>
+  <si>
+    <t>Questions seen/total: 55.36% (10820/19544)</t>
+  </si>
+  <si>
+    <t>Semantic accuracy: 72.27%  (4607/6375)</t>
+  </si>
+  <si>
+    <t>Semantic accuracy: 72.17%  (4601/6375)</t>
+  </si>
+  <si>
+    <t>Syntactic accuracy: 70.17%  (3119/4445)</t>
+  </si>
+  <si>
+    <t>Syntactic accuracy: 69.92%  (3108/4445)</t>
+  </si>
+  <si>
+    <t>Total accuracy: 71.40%  (7726/10820)</t>
+  </si>
+  <si>
+    <t>Total accuracy: 71.25%  (7709/10820)</t>
+  </si>
+  <si>
+    <t>0.44542718 0.426030748740061</t>
+  </si>
+  <si>
+    <t>[0.28633193 0.11676843 0.09353362 0.07186453 0.06552153 0.05351857 0.0471763  0.04025202 0.03875825 0.03124195]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[0.63171184 0.11711445 0.06208693 0.03295661 0.02583572 0.02417193 0.01876501 0.01722527 0.01438883 0.01111564]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[0.8134059  0.05878878 0.03315523 0.02614427 0.01813707 0.00998843 0.00779787 0.00627137 0.00506332 0.00470372]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[0.68817972 0.09736926 0.04696623 0.02594634 0.02426833 0.02200869 0.01670254 0.01552719 0.01180113 0.01062583]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wordsim-353(pearsonr, spearmanr)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>simverb-3500(pearsonr, spearmanr)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.47189963 0.45417403494167746</t>
+  </si>
+  <si>
+    <t>0.7434401839819833 0.7890802278376934(329 pairs)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -122,8 +279,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -404,77 +564,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
+    <col min="2" max="2" width="36.75" customWidth="1"/>
+    <col min="3" max="3" width="41.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
+      <c r="F3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -482,4 +658,281 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.375" customWidth="1"/>
+    <col min="2" max="2" width="41.125" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
The Worst-case Scenario Survival Hand-book
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="167">
   <si>
     <t>sentiment-PCA</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -526,15 +526,9 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Test accuracy: 0.87943</t>
-  </si>
-  <si>
     <t>Test accuracy: 0.88018</t>
   </si>
   <si>
-    <t>Test accuracy: 0.87250</t>
-  </si>
-  <si>
     <t>[0.97588256 0.00488805 0.00327049 0.00245558 0.00210812 0.00181584 0.00158151 0.00134564 0.00114076 0.00097626]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -543,8 +537,34 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>会摒弃诱导方向，并逐渐收敛至随机选择的新方向</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>初始化与否对结果基本无影响</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test accuracy: 0.88061</t>
+  </si>
+  <si>
+    <t>Test accuracy: 0.87641</t>
+  </si>
+  <si>
+    <t>refined-20(fastText-crawl-300d-2M.vec)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[9.81734241e-01 1.40975627e-02 3.01732784e-03 1.90421184e-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.58411093e-04 1.31437808e-04 1.13063820e-04 1.07061028e-04 9.06072057e-05 6.84664855e-05]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test accuracy: 0.87439</t>
+  </si>
+  <si>
+    <t>Test accuracy: 0.86567</t>
+  </si>
+  <si>
+    <t>Test accuracy: 0.85855</t>
   </si>
 </sst>
 </file>
@@ -872,10 +892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -883,12 +903,12 @@
     <col min="1" max="1" width="29.625" customWidth="1"/>
     <col min="2" max="2" width="36.75" customWidth="1"/>
     <col min="3" max="3" width="41.25" customWidth="1"/>
-    <col min="4" max="6" width="40.375" customWidth="1"/>
-    <col min="7" max="7" width="22.625" customWidth="1"/>
-    <col min="8" max="8" width="21.25" customWidth="1"/>
+    <col min="4" max="7" width="40.375" customWidth="1"/>
+    <col min="8" max="8" width="22.625" customWidth="1"/>
+    <col min="9" max="9" width="21.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>10</v>
       </c>
@@ -904,20 +924,23 @@
       <c r="F1" t="s">
         <v>150</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I1" t="s">
         <v>66</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -937,7 +960,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -956,17 +979,17 @@
       <c r="F3" t="s">
         <v>152</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>3</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>4</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -986,36 +1009,36 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>62</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>63</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1034,17 +1057,25 @@
       <c r="F10" t="s">
         <v>154</v>
       </c>
-      <c r="I10" t="s">
+      <c r="G10" t="s">
+        <v>162</v>
+      </c>
+      <c r="J10" t="s">
         <v>59</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>60</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>110</v>
       </c>
@@ -1054,11 +1085,11 @@
       <c r="C12" t="s">
         <v>67</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>0.88866999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>73</v>
       </c>
@@ -1066,7 +1097,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>74</v>
       </c>
@@ -1074,7 +1105,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>75</v>
       </c>
@@ -1082,7 +1113,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>76</v>
       </c>
@@ -1090,7 +1121,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>111</v>
       </c>
@@ -1107,13 +1143,16 @@
         <v>104</v>
       </c>
       <c r="F19" t="s">
-        <v>155</v>
-      </c>
-      <c r="H19" t="s">
+        <v>159</v>
+      </c>
+      <c r="G19" t="s">
+        <v>94</v>
+      </c>
+      <c r="I19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>113</v>
       </c>
@@ -1127,13 +1166,16 @@
         <v>105</v>
       </c>
       <c r="F20" t="s">
-        <v>156</v>
-      </c>
-      <c r="H20" t="s">
+        <v>160</v>
+      </c>
+      <c r="G20" t="s">
+        <v>155</v>
+      </c>
+      <c r="I20" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>115</v>
       </c>
@@ -1146,14 +1188,14 @@
       <c r="E21" t="s">
         <v>106</v>
       </c>
-      <c r="F21" t="s">
-        <v>157</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="G21" t="s">
+        <v>164</v>
+      </c>
+      <c r="I21" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>116</v>
       </c>
@@ -1166,11 +1208,14 @@
       <c r="E22" t="s">
         <v>107</v>
       </c>
-      <c r="H22" t="s">
+      <c r="G22" t="s">
+        <v>165</v>
+      </c>
+      <c r="I22" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>117</v>
       </c>
@@ -1183,11 +1228,14 @@
       <c r="E23" t="s">
         <v>112</v>
       </c>
-      <c r="H23" t="s">
+      <c r="G23" t="s">
+        <v>166</v>
+      </c>
+      <c r="I23" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>109</v>
       </c>
@@ -1197,11 +1245,11 @@
       <c r="C25" t="s">
         <v>82</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>108</v>
       </c>
@@ -1212,21 +1260,21 @@
         <v>85</v>
       </c>
       <c r="F26" t="s">
-        <v>158</v>
-      </c>
-      <c r="H26" t="s">
+        <v>156</v>
+      </c>
+      <c r="G26" t="s">
+        <v>156</v>
+      </c>
+      <c r="I26" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>159</v>
-      </c>
-      <c r="F30" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>124</v>
       </c>
@@ -1243,10 +1291,13 @@
         <v>0.38729708855902201</v>
       </c>
       <c r="F31">
-        <v>0.15569407809799099</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+        <v>-0.492624995588681</v>
+      </c>
+      <c r="G31">
+        <v>-0.50195767182505602</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B32">
         <v>-0.20782714416994899</v>
       </c>
@@ -1260,10 +1311,13 @@
         <v>0.36919756785503</v>
       </c>
       <c r="F32">
-        <v>0.14496865137284501</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.46686488611166099</v>
+      </c>
+      <c r="G32">
+        <v>0.47431267647700298</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B33">
         <v>-0.206482390481981</v>
       </c>
@@ -1276,11 +1330,11 @@
       <c r="E33">
         <v>-0.37015823868810499</v>
       </c>
-      <c r="F33">
-        <v>-0.143938637620904</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <v>0.47911675949471899</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B34">
         <v>-0.20758430284377299</v>
       </c>
@@ -1293,8 +1347,11 @@
       <c r="E34">
         <v>0.398434294553354</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <v>-0.48641435950406198</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B35">
         <v>0.20801400777731599</v>
       </c>
@@ -1307,8 +1364,11 @@
       <c r="E35">
         <v>0.40645602168640499</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35">
+        <v>-0.49437183936504397</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>130</v>
       </c>
@@ -1325,7 +1385,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>146</v>
       </c>
@@ -1339,7 +1399,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>147</v>
       </c>

</xml_diff>

<commit_message>
Using tensorlayer to implement naive-lstm
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="175">
   <si>
     <t>sentiment-PCA</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -584,6 +584,38 @@
   </si>
   <si>
     <t>dire_vertical_to_mean 0.80590 减去一个无关紧要的方向</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test accuracy: 0.86850</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test accuracy: 0.86619</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test accuracy: 0.85289</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test accuracy: 0.85671</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test accuracy: 0.86194</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test accuracy: 0.86011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test accuracy: 0.84974</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test accuracy: 0.84238</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -912,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" topLeftCell="B67" workbookViewId="0">
+      <selection activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1403,6 +1435,63 @@
     <row r="53" spans="2:7" x14ac:dyDescent="0.2">
       <c r="G53" t="s">
         <v>166</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B86" t="s">
+        <v>9</v>
+      </c>
+      <c r="C86" t="s">
+        <v>78</v>
+      </c>
+      <c r="D86" t="s">
+        <v>79</v>
+      </c>
+      <c r="E86" t="s">
+        <v>80</v>
+      </c>
+      <c r="F86" t="s">
+        <v>107</v>
+      </c>
+      <c r="G86" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>84</v>
+      </c>
+      <c r="D87" t="s">
+        <v>170</v>
+      </c>
+      <c r="G87" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D88" t="s">
+        <v>171</v>
+      </c>
+      <c r="G88" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D89" t="s">
+        <v>172</v>
+      </c>
+      <c r="G89" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D90" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D91" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>